<commit_message>
Career Guidance Full Stack Developer
</commit_message>
<xml_diff>
--- a/Technical_Skill_Upgrade.xlsx
+++ b/Technical_Skill_Upgrade.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/mradhakrish9_dxc_com/Documents/Monica/Skill-Upgrade-Oct'23/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/mradhakrish9_dxc_com/Documents/Monica/Skill-Upgrade-Oct'23/Java_Full_Stack/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="569" documentId="11_F25DC773A252ABDACC104890895F6D105BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF3951AE-6319-4339-960A-3B70BE4D3B78}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Interview_Pattern" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1037,96 +1037,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1137,6 +1047,108 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1146,25 +1158,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1781,52 +1781,52 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="44">
+      <c r="A2" s="42">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="34">
+      <c r="C2" s="46">
         <v>45090</v>
       </c>
-      <c r="D2" s="37">
+      <c r="D2" s="49">
         <v>45120</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="27"/>
+      <c r="E2" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="59"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="45"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="29"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="61"/>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="46"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="30"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="62"/>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="47"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="28"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="60"/>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6"/>
@@ -1837,42 +1837,42 @@
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="44">
+      <c r="A7" s="42">
         <v>2</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="46">
         <v>45121</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="49">
         <v>45152</v>
       </c>
-      <c r="E7" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="27"/>
+      <c r="E7" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="59"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="45"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="29"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="61"/>
     </row>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="47"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="28"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="60"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="6"/>
@@ -1883,42 +1883,42 @@
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="44">
+      <c r="A11" s="42">
         <v>3</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="46">
         <v>45153</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="49">
         <v>45184</v>
       </c>
-      <c r="E11" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="27"/>
+      <c r="E11" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="59"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="45"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="29"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="61"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="47"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="28"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="60"/>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="6"/>
@@ -1929,42 +1929,42 @@
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="44">
+      <c r="A15" s="42">
         <v>4</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="46">
         <v>45185</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="49">
         <v>45215</v>
       </c>
-      <c r="E15" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="27"/>
+      <c r="E15" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="59"/>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="45"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="29"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="61"/>
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="47"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="28"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="60"/>
     </row>
     <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="6"/>
@@ -1975,32 +1975,32 @@
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="44">
+      <c r="A19" s="42">
         <v>5</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="46">
         <v>45216</v>
       </c>
-      <c r="D19" s="37">
+      <c r="D19" s="49">
         <v>45247</v>
       </c>
-      <c r="E19" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="27"/>
+      <c r="E19" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="59"/>
     </row>
     <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="47"/>
+      <c r="A20" s="45"/>
       <c r="B20" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="28"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="60"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
@@ -2012,11 +2012,14 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="C19:C20"/>
@@ -2029,14 +2032,11 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A19:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2166,7 +2166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2AB7B4-917E-4677-9338-8FBEA8425047}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B20" sqref="B20:B27"/>
     </sheetView>
   </sheetViews>
@@ -2193,10 +2193,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="51">
+      <c r="A2" s="63">
         <v>1</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="66" t="s">
         <v>84</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -2205,26 +2205,26 @@
       <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="52"/>
-      <c r="B3" s="49"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="67"/>
       <c r="C3" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="53"/>
-      <c r="B4" s="50"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="68"/>
       <c r="C4" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="21"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="51">
+      <c r="A5" s="63">
         <v>2</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="66" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="17" t="s">
@@ -2233,34 +2233,34 @@
       <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="52"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="52"/>
-      <c r="B7" s="49"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="19"/>
     </row>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="53"/>
-      <c r="B8" s="50"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="20" t="s">
         <v>58</v>
       </c>
       <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="51">
+      <c r="A9" s="63">
         <v>3</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="66" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="17" t="s">
@@ -2269,58 +2269,58 @@
       <c r="D9" s="18"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="52"/>
-      <c r="B10" s="49"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="52"/>
-      <c r="B11" s="49"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D11" s="19"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="52"/>
-      <c r="B12" s="49"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D12" s="19"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="52"/>
-      <c r="B13" s="49"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D13" s="19"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="52"/>
-      <c r="B14" s="49"/>
+      <c r="A14" s="64"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="53"/>
-      <c r="B15" s="50"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="68"/>
       <c r="C15" s="20" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="51">
+      <c r="A16" s="63">
         <v>4</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="66" t="s">
         <v>65</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -2329,34 +2329,34 @@
       <c r="D16" s="18"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="52"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="64"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="19"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="52"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="64"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D18" s="19"/>
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="53"/>
-      <c r="B19" s="50"/>
+      <c r="A19" s="65"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="20" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="21"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="51">
+      <c r="A20" s="63">
         <v>5</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="66" t="s">
         <v>67</v>
       </c>
       <c r="C20" s="17" t="s">
@@ -2365,56 +2365,56 @@
       <c r="D20" s="18"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="52"/>
-      <c r="B21" s="49"/>
+      <c r="A21" s="64"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D21" s="19"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="52"/>
-      <c r="B22" s="49"/>
+      <c r="A22" s="64"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D22" s="19"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="52"/>
-      <c r="B23" s="49"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D23" s="19"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="52"/>
-      <c r="B24" s="49"/>
+      <c r="A24" s="64"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="19"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="52"/>
-      <c r="B25" s="49"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D25" s="19"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="52"/>
-      <c r="B26" s="49"/>
+      <c r="A26" s="64"/>
+      <c r="B26" s="67"/>
       <c r="C26" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D26" s="19"/>
     </row>
     <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="53"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="65"/>
+      <c r="B27" s="68"/>
       <c r="C27" s="20" t="s">
         <v>75</v>
       </c>
@@ -2433,10 +2433,10 @@
       <c r="D28" s="25"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="51">
+      <c r="A29" s="63">
         <v>7</v>
       </c>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="66" t="s">
         <v>78</v>
       </c>
       <c r="C29" s="17" t="s">
@@ -2445,104 +2445,104 @@
       <c r="D29" s="18"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="52"/>
-      <c r="B30" s="49"/>
+      <c r="A30" s="64"/>
+      <c r="B30" s="67"/>
       <c r="C30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="19"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="52"/>
-      <c r="B31" s="49"/>
+      <c r="A31" s="64"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="19"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="52"/>
-      <c r="B32" s="49"/>
+      <c r="A32" s="64"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="19"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="52"/>
-      <c r="B33" s="49"/>
+      <c r="A33" s="64"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="19"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="52"/>
-      <c r="B34" s="49"/>
+      <c r="A34" s="64"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D34" s="19"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="52"/>
-      <c r="B35" s="49"/>
+      <c r="A35" s="64"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="19"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="52"/>
-      <c r="B36" s="49"/>
+      <c r="A36" s="64"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="15" t="s">
         <v>25</v>
       </c>
       <c r="D36" s="19"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="52"/>
-      <c r="B37" s="49"/>
+      <c r="A37" s="64"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D37" s="19"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="52"/>
-      <c r="B38" s="49"/>
+      <c r="A38" s="64"/>
+      <c r="B38" s="67"/>
       <c r="C38" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D38" s="19"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="52"/>
-      <c r="B39" s="49"/>
+      <c r="A39" s="64"/>
+      <c r="B39" s="67"/>
       <c r="C39" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D39" s="19"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="52"/>
-      <c r="B40" s="49"/>
+      <c r="A40" s="64"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D40" s="19"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="52"/>
-      <c r="B41" s="49"/>
+      <c r="A41" s="64"/>
+      <c r="B41" s="67"/>
       <c r="C41" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D41" s="19"/>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="53"/>
-      <c r="B42" s="50"/>
+      <c r="A42" s="65"/>
+      <c r="B42" s="68"/>
       <c r="C42" s="26" t="s">
         <v>85</v>
       </c>
@@ -2550,11 +2550,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="B9:B15"/>
     <mergeCell ref="B29:B42"/>
     <mergeCell ref="A29:A42"/>
     <mergeCell ref="A20:A27"/>
@@ -2562,6 +2557,11 @@
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="B20:B27"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B9:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2572,8 +2572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C14826-1E89-468B-8550-BACA1C89B181}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2587,418 +2587,418 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="36" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="54">
+      <c r="A2" s="72">
         <v>1</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="72" t="s">
         <v>86</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="72" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="65" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="69" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
+      <c r="A3" s="73"/>
+      <c r="B3" s="73"/>
       <c r="C3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="66"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="70"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="54">
+      <c r="A4" s="72">
         <v>2</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="72" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="72" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="66"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="70"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="56"/>
-      <c r="B5" s="56"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="66"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="70"/>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="55"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="61"/>
-      <c r="E6" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="66"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="70"/>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="71">
+      <c r="A7" s="38">
         <v>3</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="57" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="66"/>
+      <c r="E7" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="70"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="54">
+      <c r="A8" s="72">
         <v>4</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="72" t="s">
         <v>96</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="72" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="66"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="70"/>
     </row>
     <row r="9" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="56"/>
-      <c r="B9" s="56"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="66"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="70"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="56"/>
-      <c r="B10" s="56"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="66"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="70"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="56"/>
-      <c r="B11" s="56"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="66"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="70"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="56"/>
-      <c r="B12" s="56"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="66"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="70"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="55"/>
-      <c r="B13" s="55"/>
+      <c r="A13" s="73"/>
+      <c r="B13" s="73"/>
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="61"/>
-      <c r="E13" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="66"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="70"/>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="57">
+      <c r="A14" s="27">
         <v>5</v>
       </c>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="27" t="s">
         <v>102</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="64"/>
-      <c r="E14" s="57" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="66"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="70"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="57">
+      <c r="A15" s="27">
         <v>6</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="27" t="s">
         <v>68</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="64"/>
-      <c r="E15" s="57" t="s">
+      <c r="D15" s="34"/>
+      <c r="E15" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="F15" s="66"/>
+      <c r="F15" s="70"/>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="57">
+      <c r="A16" s="27">
         <v>7</v>
       </c>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="27" t="s">
         <v>105</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="57" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="66"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="70"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="54">
+      <c r="A17" s="72">
         <v>8</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="72" t="s">
         <v>107</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="62"/>
-      <c r="E17" s="72" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="66"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="70"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="56"/>
-      <c r="B18" s="56"/>
+      <c r="A18" s="74"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="63"/>
-      <c r="E18" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="66"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="70"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="56"/>
-      <c r="B19" s="56"/>
+      <c r="A19" s="74"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="63"/>
-      <c r="E19" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="66"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="70"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="56"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="59" t="s">
+      <c r="A20" s="74"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="63" t="s">
+      <c r="D20" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="E20" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="66"/>
+      <c r="E20" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="70"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="56"/>
-      <c r="B21" s="56"/>
+      <c r="A21" s="74"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="63"/>
-      <c r="E21" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="66"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="70"/>
     </row>
     <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="55"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="60" t="s">
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="61" t="s">
+      <c r="D22" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="E22" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="66"/>
+      <c r="E22" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="70"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="54">
+      <c r="A23" s="72">
         <v>9</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="72" t="s">
         <v>113</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="72" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="66"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="70"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="56"/>
-      <c r="B24" s="56"/>
+      <c r="A24" s="74"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="63"/>
-      <c r="E24" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="66"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="70"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="56"/>
-      <c r="B25" s="56"/>
+      <c r="A25" s="74"/>
+      <c r="B25" s="74"/>
       <c r="C25" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="66"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="70"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="56"/>
-      <c r="B26" s="56"/>
+      <c r="A26" s="74"/>
+      <c r="B26" s="74"/>
       <c r="C26" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="63"/>
-      <c r="E26" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="66"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="70"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="56"/>
-      <c r="B27" s="56"/>
+      <c r="A27" s="74"/>
+      <c r="B27" s="74"/>
       <c r="C27" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="63"/>
-      <c r="E27" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="66"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="70"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="56"/>
-      <c r="B28" s="56"/>
+      <c r="A28" s="74"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="63"/>
-      <c r="E28" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="66"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="70"/>
     </row>
     <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="55"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="73"/>
+      <c r="B29" s="73"/>
       <c r="C29" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="61"/>
-      <c r="E29" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="67"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A23:A29"/>
     <mergeCell ref="F2:F29"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="B17:B22"/>
     <mergeCell ref="B23:B29"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="A23:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
JDBC Servlets and JSP
</commit_message>
<xml_diff>
--- a/Technical_Skill_Upgrade.xlsx
+++ b/Technical_Skill_Upgrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/mradhakrish9_dxc_com/Documents/Monica/Skill-Upgrade-Oct'23/Java_Full_Stack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="574" documentId="11_F25DC773A252ABDACC104890895F6D105BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E564DE8A-B94E-4FFC-B715-5FFECD488BD5}"/>
+  <xr:revisionPtr revIDLastSave="580" documentId="11_F25DC773A252ABDACC104890895F6D105BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CE42B0B-3817-4240-900C-1E0C8235BE80}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Interview_Pattern" sheetId="1" state="hidden" r:id="rId1"/>
@@ -996,7 +996,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1020,9 +1020,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1035,7 +1034,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1076,6 +1074,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1106,10 +1107,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1124,9 +1122,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1174,9 +1169,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1792,52 +1784,52 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="41">
+      <c r="A2" s="40">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="45">
+      <c r="C2" s="44">
         <v>45090</v>
       </c>
-      <c r="D2" s="48">
+      <c r="D2" s="47">
         <v>45120</v>
       </c>
-      <c r="E2" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="58"/>
+      <c r="E2" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="42"/>
+      <c r="A3" s="41"/>
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="60"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="57"/>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="43"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="61"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="58"/>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="44"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="59"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="56"/>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6"/>
@@ -1848,42 +1840,42 @@
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="41">
+      <c r="A7" s="40">
         <v>2</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="44">
         <v>45121</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="47">
         <v>45152</v>
       </c>
-      <c r="E7" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="58"/>
+      <c r="E7" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="55"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="42"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="60"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="57"/>
     </row>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="44"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="59"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="56"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="6"/>
@@ -1894,42 +1886,42 @@
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="41">
+      <c r="A11" s="40">
         <v>3</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="45">
+      <c r="C11" s="44">
         <v>45153</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="47">
         <v>45184</v>
       </c>
-      <c r="E11" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="58"/>
+      <c r="E11" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="55"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="42"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="60"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="57"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="44"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="59"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="56"/>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="6"/>
@@ -1940,42 +1932,42 @@
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="41">
+      <c r="A15" s="40">
         <v>4</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="44">
         <v>45185</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="47">
         <v>45215</v>
       </c>
-      <c r="E15" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="58"/>
+      <c r="E15" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="55"/>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="42"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="60"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="57"/>
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="44"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="59"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="56"/>
     </row>
     <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="6"/>
@@ -1986,32 +1978,32 @@
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="41">
+      <c r="A19" s="40">
         <v>5</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C19" s="44">
         <v>45216</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D19" s="47">
         <v>45247</v>
       </c>
-      <c r="E19" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="58"/>
+      <c r="E19" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="55"/>
     </row>
     <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="44"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="59"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="56"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
@@ -2177,14 +2169,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2AB7B4-917E-4677-9338-8FBEA8425047}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="16"/>
-    <col min="2" max="2" width="24.453125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="15"/>
+    <col min="2" max="2" width="24.453125" style="15" customWidth="1"/>
     <col min="3" max="3" width="30.90625" customWidth="1"/>
     <col min="4" max="4" width="24.90625" style="4" customWidth="1"/>
   </cols>
@@ -2204,366 +2196,366 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="62">
+      <c r="A2" s="59">
         <v>1</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="36" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="63"/>
-      <c r="B3" s="66"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="38"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="64"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="18" t="s">
+      <c r="A4" s="61"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="37"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="62">
+      <c r="A5" s="59">
         <v>2</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="63"/>
-      <c r="B6" s="66"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="40"/>
+      <c r="D6" s="38"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="63"/>
-      <c r="B7" s="66"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="40"/>
+      <c r="D7" s="38"/>
     </row>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="64"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="18" t="s">
+      <c r="A8" s="61"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="39"/>
+      <c r="D8" s="37"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="62">
+      <c r="A9" s="59">
         <v>3</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="36" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="63"/>
-      <c r="B10" s="66"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="40"/>
+      <c r="D10" s="38"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="63"/>
-      <c r="B11" s="66"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="40"/>
+      <c r="D11" s="38"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="63"/>
-      <c r="B12" s="66"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="40"/>
+      <c r="D12" s="38"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="63"/>
-      <c r="B13" s="66"/>
+      <c r="A13" s="60"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="40"/>
+      <c r="D13" s="38"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="63"/>
-      <c r="B14" s="66"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="40"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="64"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="18" t="s">
+      <c r="A15" s="61"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="39"/>
+      <c r="D15" s="37"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="62">
+      <c r="A16" s="59">
         <v>4</v>
       </c>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="38"/>
+      <c r="D16" s="36"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="63"/>
-      <c r="B17" s="66"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="40"/>
+      <c r="D17" s="38"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="63"/>
-      <c r="B18" s="66"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="40"/>
+      <c r="D18" s="38"/>
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="64"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="18" t="s">
+      <c r="A19" s="61"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="39"/>
+      <c r="D19" s="37"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="62">
+      <c r="A20" s="59">
         <v>5</v>
       </c>
-      <c r="B20" s="65" t="s">
+      <c r="B20" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="36" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="63"/>
-      <c r="B21" s="66"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="63"/>
       <c r="C21" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="40"/>
+      <c r="D21" s="38"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="63"/>
-      <c r="B22" s="66"/>
+      <c r="A22" s="60"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="40"/>
+      <c r="D22" s="38"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="63"/>
-      <c r="B23" s="66"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="63"/>
       <c r="C23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="40"/>
+      <c r="D23" s="38"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="63"/>
-      <c r="B24" s="66"/>
+      <c r="A24" s="60"/>
+      <c r="B24" s="63"/>
       <c r="C24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="40"/>
+      <c r="D24" s="38"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="63"/>
-      <c r="B25" s="66"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="40"/>
+      <c r="D25" s="38"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="63"/>
-      <c r="B26" s="66"/>
+      <c r="A26" s="60"/>
+      <c r="B26" s="63"/>
       <c r="C26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="40"/>
+      <c r="D26" s="38"/>
     </row>
     <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="64"/>
-      <c r="B27" s="67"/>
-      <c r="C27" s="18" t="s">
+      <c r="A27" s="61"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="39"/>
+      <c r="D27" s="37"/>
     </row>
     <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="19">
+      <c r="A28" s="18">
         <v>6</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="74"/>
+      <c r="D28" s="39"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="62">
+      <c r="A29" s="59">
         <v>7</v>
       </c>
-      <c r="B29" s="65" t="s">
+      <c r="B29" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="38"/>
+      <c r="D29" s="36"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="63"/>
-      <c r="B30" s="66"/>
+      <c r="A30" s="60"/>
+      <c r="B30" s="63"/>
       <c r="C30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="40"/>
+      <c r="D30" s="38"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="63"/>
-      <c r="B31" s="66"/>
+      <c r="A31" s="60"/>
+      <c r="B31" s="63"/>
       <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="40"/>
+      <c r="D31" s="38"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="63"/>
-      <c r="B32" s="66"/>
+      <c r="A32" s="60"/>
+      <c r="B32" s="63"/>
       <c r="C32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="40"/>
+      <c r="D32" s="38"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="63"/>
-      <c r="B33" s="66"/>
+      <c r="A33" s="60"/>
+      <c r="B33" s="63"/>
       <c r="C33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="40"/>
+      <c r="D33" s="38"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="63"/>
-      <c r="B34" s="66"/>
+      <c r="A34" s="60"/>
+      <c r="B34" s="63"/>
       <c r="C34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="40"/>
+      <c r="D34" s="38"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="63"/>
-      <c r="B35" s="66"/>
+      <c r="A35" s="60"/>
+      <c r="B35" s="63"/>
       <c r="C35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="40"/>
+      <c r="D35" s="38"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="63"/>
-      <c r="B36" s="66"/>
-      <c r="C36" s="15" t="s">
+      <c r="A36" s="60"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="40"/>
+      <c r="D36" s="38"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="63"/>
-      <c r="B37" s="66"/>
+      <c r="A37" s="60"/>
+      <c r="B37" s="63"/>
       <c r="C37" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="40"/>
+      <c r="D37" s="38"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="63"/>
-      <c r="B38" s="66"/>
+      <c r="A38" s="60"/>
+      <c r="B38" s="63"/>
       <c r="C38" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="40"/>
+      <c r="D38" s="38"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="63"/>
-      <c r="B39" s="66"/>
+      <c r="A39" s="60"/>
+      <c r="B39" s="63"/>
       <c r="C39" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="40"/>
+      <c r="D39" s="38"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="63"/>
-      <c r="B40" s="66"/>
+      <c r="A40" s="60"/>
+      <c r="B40" s="63"/>
       <c r="C40" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D40" s="40"/>
+      <c r="D40" s="38"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="63"/>
-      <c r="B41" s="66"/>
+      <c r="A41" s="60"/>
+      <c r="B41" s="63"/>
       <c r="C41" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="40"/>
+      <c r="D41" s="38"/>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="64"/>
-      <c r="B42" s="67"/>
-      <c r="C42" s="22" t="s">
+      <c r="A42" s="61"/>
+      <c r="B42" s="64"/>
+      <c r="C42" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="D42" s="39"/>
+      <c r="D42" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2589,419 +2581,419 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C14826-1E89-468B-8550-BACA1C89B181}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="16"/>
-    <col min="2" max="2" width="17.81640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="15"/>
+    <col min="2" max="2" width="17.81640625" style="15" customWidth="1"/>
     <col min="3" max="3" width="49.453125" customWidth="1"/>
     <col min="4" max="4" width="53.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" style="15" customWidth="1"/>
     <col min="6" max="6" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="30" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="71">
+      <c r="A2" s="68">
         <v>1</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="68" t="s">
         <v>86</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="68" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="65" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="72"/>
-      <c r="B3" s="72"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="69"/>
       <c r="C3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="69"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="66"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="71">
+      <c r="A4" s="68">
         <v>2</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="68" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="69"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="66"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="73"/>
-      <c r="B5" s="73"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="69"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="66"/>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="72"/>
-      <c r="B6" s="72"/>
+      <c r="A6" s="69"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="69"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="66"/>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="34">
+      <c r="A7" s="32">
         <v>3</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="69"/>
+      <c r="E7" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="66"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="71">
+      <c r="A8" s="68">
         <v>4</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="68" t="s">
         <v>96</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="69"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="66"/>
     </row>
     <row r="9" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="73"/>
-      <c r="B9" s="73"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="69"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="66"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="73"/>
-      <c r="B10" s="73"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="70"/>
       <c r="C10" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="69"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="66"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="73"/>
-      <c r="B11" s="73"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="69"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="66"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="73"/>
-      <c r="B12" s="73"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="69"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="66"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="72"/>
-      <c r="B13" s="72"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="69"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="66"/>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="23">
+      <c r="A14" s="21">
         <v>5</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="21" t="s">
         <v>102</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="69"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="66"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="23">
+      <c r="A15" s="21">
         <v>6</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="21" t="s">
         <v>68</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="23" t="s">
+      <c r="D15" s="28"/>
+      <c r="E15" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="F15" s="69"/>
+      <c r="F15" s="66"/>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="23">
+      <c r="A16" s="21">
         <v>7</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="21" t="s">
         <v>105</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="69"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="66"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="71">
+      <c r="A17" s="68">
         <v>8</v>
       </c>
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="68" t="s">
         <v>107</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="69"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="66"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="73"/>
-      <c r="B18" s="73"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="70"/>
       <c r="C18" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="69"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="66"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="70"/>
       <c r="C19" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="69"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="66"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
-      <c r="C20" s="25" t="s">
+      <c r="A20" s="70"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="E20" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="69"/>
+      <c r="E20" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="66"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="70"/>
       <c r="C21" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="29"/>
-      <c r="E21" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="69"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="66"/>
     </row>
     <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="72"/>
-      <c r="B22" s="72"/>
-      <c r="C22" s="26" t="s">
+      <c r="A22" s="69"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="E22" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="69"/>
+      <c r="E22" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="66"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="71">
+      <c r="A23" s="68">
         <v>9</v>
       </c>
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="68" t="s">
         <v>113</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="69"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="66"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="73"/>
-      <c r="B24" s="73"/>
+      <c r="A24" s="70"/>
+      <c r="B24" s="70"/>
       <c r="C24" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="69"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="66"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="73"/>
-      <c r="B25" s="73"/>
+      <c r="A25" s="70"/>
+      <c r="B25" s="70"/>
       <c r="C25" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="29"/>
-      <c r="E25" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="69"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="66"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="73"/>
-      <c r="B26" s="73"/>
+      <c r="A26" s="70"/>
+      <c r="B26" s="70"/>
       <c r="C26" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="29"/>
-      <c r="E26" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="69"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="66"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="73"/>
-      <c r="B27" s="73"/>
+      <c r="A27" s="70"/>
+      <c r="B27" s="70"/>
       <c r="C27" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="29"/>
-      <c r="E27" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="69"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="66"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="70"/>
+      <c r="B28" s="70"/>
       <c r="C28" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="69"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="66"/>
     </row>
     <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="72"/>
-      <c r="B29" s="72"/>
+      <c r="A29" s="69"/>
+      <c r="B29" s="69"/>
       <c r="C29" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="70"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>